<commit_message>
feat : output file improve, syntax improvement
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Quantité</t>
   </si>
@@ -44,13 +44,13 @@
     <t>test</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse de l'Association (partie 1)</t>
+    <t xml:space="preserve">Adresse de l'association (partie 1)</t>
   </si>
   <si>
     <t xml:space="preserve">2 rue Charles Camichel</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse de l'Association (partie 2)</t>
+    <t xml:space="preserve">Adresse de l'association (partie 2)</t>
   </si>
   <si>
     <t xml:space="preserve">31071 Toulouse CEDEX 7</t>
@@ -62,6 +62,30 @@
     <t>Toulouse</t>
   </si>
   <si>
+    <t xml:space="preserve">Nom de l'association</t>
+  </si>
+  <si>
+    <t>Wallstreet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email de l'association</t>
+  </si>
+  <si>
+    <t>jordan.belfort@gmail.com</t>
+  </si>
+  <si>
+    <t>Mandat</t>
+  </si>
+  <si>
+    <t>2025-2026</t>
+  </si>
+  <si>
+    <t>Trésorier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jordan Belfort</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nom du fichier logo (vide si pas)</t>
   </si>
   <si>
@@ -86,6 +110,12 @@
     <t xml:space="preserve">Virement bancaire</t>
   </si>
   <si>
+    <t xml:space="preserve">Noms pièces jointes (séparées par une virgule)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Numéro de la note de frais</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adresse (partie 1)</t>
   </si>
   <si>
@@ -96,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">IBAN (remplissage auto à partir du bénéficiaire)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Noms pièces jointes (une par ligne vers le bas)</t>
   </si>
   <si>
     <t xml:space="preserve">Prénom Nom</t>
@@ -132,7 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.000000"/>
       <color theme="1"/>
@@ -152,6 +179,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11.000000"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -180,15 +213,16 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -758,7 +792,7 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="5" t="s">
@@ -766,7 +800,7 @@
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -774,18 +808,18 @@
       </c>
     </row>
     <row r="7" ht="14.25">
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -793,59 +827,96 @@
       <c r="F9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G9" s="7" t="str">
-        <f>_xlfn.XLOOKUP(G7,Bénéficiaires!A:A,Bénéficiaires!B:B,"Adresse non-renseignée")</f>
-        <v xml:space="preserve">200 rue du Basket</v>
+      <c r="G9" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" ht="14.25">
       <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="8" t="str">
-        <f>_xlfn.XLOOKUP(G7,Bénéficiaires!A:A,Bénéficiaires!C:C,"Adresse non-renseignée")</f>
-        <v xml:space="preserve">31000 Toulouse</v>
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="11" ht="14.25">
-      <c r="F11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="8" t="str">
-        <f>_xlfn.XLOOKUP(G7,Bénéficiaires!A:A,Bénéficiaires!D:D,"Téléphone non-renseigné")</f>
-        <v xml:space="preserve">06 69 69 69 69</v>
+      <c r="F11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" ht="14.25">
-      <c r="F12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" t="str">
-        <f>IF(G8="Virement bancaire",_xlfn.XLOOKUP(G7,Bénéficiaires!A:A,Bénéficiaires!E:E,"IBAN non-renseigné"),"")</f>
-        <v xml:space="preserve">FR76 0000 0000 5700 0408 9597 000</v>
+      <c r="F12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="13" ht="14.25">
       <c r="F13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="G13" s="8"/>
     </row>
     <row r="14" ht="14.25">
-      <c r="G14" s="6"/>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" ht="14.25">
-      <c r="G15" s="6"/>
+      <c r="F15" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" s="9" t="str">
+        <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!B:B,"Adresse non-renseignée")</f>
+        <v xml:space="preserve">200 rue du Basket</v>
+      </c>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="F16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" s="5" t="str">
+        <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!C:C,"Adresse non-renseignée")</f>
+        <v xml:space="preserve">31000 Toulouse</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="F17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="5" t="str">
+        <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!D:D,"Téléphone non-renseigné")</f>
+        <v xml:space="preserve">06 69 69 69 69</v>
+      </c>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="F18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G18" t="str">
+        <f>IF(G12="Virement bancaire",_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!E:E,"IBAN non-renseigné"),"")</f>
+        <v xml:space="preserve">FR76 0000 0000 5700 0408 9597 000</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2" disablePrompts="0">
-    <dataValidation sqref="G7" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" promptTitle="" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+    <dataValidation sqref="G11" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" promptTitle="" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Bénéficiaires!$A$2:$A$1000</formula1>
     </dataValidation>
-    <dataValidation sqref="G8" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
+    <dataValidation sqref="G12" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="1">
       <formula1>Options!$A$2:$A$4</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="G6"/>
+  </hyperlinks>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="0" copies="1"/>
@@ -870,36 +941,36 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>32</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -929,22 +1000,22 @@
   <sheetData>
     <row r="1" ht="14.25">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" ht="14.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="14.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: improvement of variable names and global structure
</commit_message>
<xml_diff>
--- a/assets/data.xlsx
+++ b/assets/data.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Options" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bénéficiaires!$A$1:$E$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Bénéficiaires!$A$1:$E$2</definedName>
   </definedNames>
   <calcPr/>
@@ -213,18 +214,16 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
+      <protection hidden="0" locked="1"/>
+    </xf>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -776,7 +775,11 @@
       </c>
     </row>
     <row r="3" ht="14.25">
-      <c r="F3" s="4" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
@@ -784,7 +787,11 @@
       </c>
     </row>
     <row r="4" ht="14.25">
-      <c r="F4" s="4" t="s">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="G4" t="s">
@@ -792,22 +799,34 @@
       </c>
     </row>
     <row r="5" ht="14.25">
-      <c r="F5" s="4" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="F5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" ht="14.25">
-      <c r="F6" s="4" t="s">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="5" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" ht="14.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
       <c r="F7" s="2" t="s">
         <v>17</v>
       </c>
@@ -816,10 +835,14 @@
       </c>
     </row>
     <row r="8" ht="14.25">
-      <c r="F8" s="4" t="s">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="F8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G8" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -843,7 +866,7 @@
       <c r="F11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="6" t="s">
         <v>26</v>
       </c>
     </row>
@@ -851,7 +874,7 @@
       <c r="F12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="6" t="s">
         <v>28</v>
       </c>
     </row>
@@ -859,13 +882,13 @@
       <c r="F13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" ht="14.25">
       <c r="F14" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="7">
+      <c r="G14" s="6">
         <v>1</v>
       </c>
     </row>
@@ -873,7 +896,7 @@
       <c r="F15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G15" s="9" t="str">
+      <c r="G15" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!B:B,"Adresse non-renseignée")</f>
         <v xml:space="preserve">200 rue du Basket</v>
       </c>
@@ -882,7 +905,7 @@
       <c r="F16" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G16" s="5" t="str">
+      <c r="G16" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!C:C,"Adresse non-renseignée")</f>
         <v xml:space="preserve">31000 Toulouse</v>
       </c>
@@ -891,7 +914,7 @@
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G17" s="5" t="str">
+      <c r="G17" s="3" t="str">
         <f>_xlfn.XLOOKUP(G11,Bénéficiaires!A:A,Bénéficiaires!D:D,"Téléphone non-renseigné")</f>
         <v xml:space="preserve">06 69 69 69 69</v>
       </c>
@@ -946,7 +969,7 @@
       <c r="B1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D1" s="1" t="s">

</xml_diff>